<commit_message>
Script finalizado. Adicionado try e axcept para tratar possíveis erros ao buscar os valores. É feito o comparativo de preços é enviando um email avisando da diferença de preço.
</commit_message>
<xml_diff>
--- a/Produtos.xlsx
+++ b/Produtos.xlsx
@@ -1,103 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Python Impressionador\Projeto_PrecosAmazon\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9A80E3-7ED9-4EE6-B66F-2E231D2FE6D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Link Produto</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>Lojas Americanas</t>
-  </si>
-  <si>
-    <t>Magazine Luiza</t>
-  </si>
-  <si>
-    <t>Preço Original</t>
-  </si>
-  <si>
-    <t>Preço Atual</t>
-  </si>
-  <si>
-    <t>Local</t>
-  </si>
-  <si>
-    <t>iPhone 11 Apple 64GB Preto</t>
-  </si>
-  <si>
-    <t>Smart TV LED 50'' LG Ultra HD 4K Thinq AI</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com.br/IPHONE-11-PRETO-TELA-C%C3%82MERA/dp/B086VQTMPR/ref=sr_1_1?__mk_pt_BR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=iphone+11&amp;qid=1606856566&amp;sr=8-1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com.br/Smart-LG-Intelig%C3%AAncia-Artificial-Virtual/dp/B0877QDB3V/ref=sr_1_1?__mk_pt_BR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=televis%C3%A3o&amp;qid=1606856629&amp;sr=8-1</t>
-  </si>
-  <si>
-    <t>https://www.americanas.com.br/produto/1611315933?pfm_carac=iphone-11-64gb-preto-ios-4g-camera-12mp-apple&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
-  </si>
-  <si>
-    <t>https://www.americanas.com.br/produto/495161500?pfm_carac=smart-tv-led-pro-50-ultra-hd-4k-lg&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
-  </si>
-  <si>
-    <t>https://www.magazineluiza.com.br/iphone-11-apple-64gb-preto-61-12mp-ios/p/155610500/te/ip11/</t>
-  </si>
-  <si>
-    <t>https://www.magazineluiza.com.br/smart-tv-uhd-4k-led-50-lg-50un7310psc-wi-fi-bluetooth-inteligencia-artificial-3-hdmi-2-usb/p/225376700/et/elit/?origin=autocomplete&amp;p=Smart%20TV%20LED%20PRO%2050%20Ultra%20HD%204K%20LG&amp;ranking=1&amp;typeclick=3&amp;ac_pos=header</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -112,54 +46,98 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -201,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,27 +211,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,24 +245,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,79 +420,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Link Produto</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Lojas Americanas</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Magazine Luiza</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Preço Original</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Preço Atual</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>iPhone 11 Apple 64GB Preto</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Iphone-Apple-Preto-128gb-Desbloqueado/dp/B07Z5HK9DC/ref=sr_1_3?__mk_pt_BR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=J2CSH6EQDKMQ&amp;keywords=iphone+11+preto+128gb&amp;qid=1638716699&amp;sprefix=iphone+11+preto+128%2Caps%2C323&amp;sr=8-3&amp;ufe=app_do%3Aamzn1.fos.25548f35-0de7-44b3-b28e-0f56f3f96147</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://www.americanas.com.br/produto/1611318018?pfm_carac=iphone-11-preto-128gb&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page&amp;offerId=5e8b830279bf8430cb9e9aae</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://www.magazineluiza.com.br/iphone-11-apple-64gb-preto-61-12mp-ios/p/155610500/te/ip11/</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>5297</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4139.1</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Magazine Luiza</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>5297</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>iPhone 12 Apple 64GB Preto 6,1” 12MP iOS</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Apple-iPhone-12-128-GB-Preto/dp/B09B49KYCW/ref=sr_1_1?__mk_pt_BR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=iphone%2B12%2Bpreto%2B128gb&amp;qid=1638716793&amp;sr=8-1&amp;ufe=app_do%3Aamzn1.fos.25548f35-0de7-44b3-b28e-0f56f3f96147&amp;th=1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://www.americanas.com.br/produto/3591024089?pfm_carac=iphone-12-preto-128gb&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page&amp;offerId=611fcf1709c351890d55d3b3&amp;buyboxToken=smartbuybox-acom-v2-61f0da6b-65a0-4592-86d2-284b1d9a8652-2021-12-05%2012%3A06%3A59-0300&amp;cor=PRETO</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.magazineluiza.com.br/iphone-12-mini-apple-128gb-preto-54-cam-dupla-12mp-ios/p/155594500/te/tcsp/</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
         <v>2900</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2900</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Preço Original</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>